<commit_message>
planejamento da sprint atualizado
</commit_message>
<xml_diff>
--- a/Documentacao/Sprints TIS III-noite-2sem2022.xlsx
+++ b/Documentacao/Sprints TIS III-noite-2sem2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\repository\plf-es-2022-2-ti3-6654100-studio-academia\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D879212-4862-49CC-9D3B-255AD7D91734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8081C94-F960-4D8B-8D47-3C1E29DD2E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados do Projeto" sheetId="1" r:id="rId1"/>
@@ -377,7 +377,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="116">
   <si>
     <t>PONTIFÍCIA UNIVERSIDADE CATÓLICA DE MINAS GERAIS</t>
   </si>
@@ -676,11 +676,6 @@
     <t>login no sistema</t>
   </si>
   <si>
-    <t>Marcos Felipe (back-end)
-Arthur Avelar (back-end)
-Arthur Alexi( front)</t>
-  </si>
-  <si>
     <t>30h</t>
   </si>
   <si>
@@ -716,6 +711,70 @@
   <si>
     <t>10h</t>
   </si>
+  <si>
+    <t>Marcos Felipe</t>
+  </si>
+  <si>
+    <t>Arthur Alex
+Ygor</t>
+  </si>
+  <si>
+    <t>Marcos Felipe (back-end)
+Arthur Avelar (Documentaçao)
+Arthur Alexi( front)
+Ygor (front)</t>
+  </si>
+  <si>
+    <t>Arthur Alexi( front)
+Ygor (front)</t>
+  </si>
+  <si>
+    <t>documentaçao</t>
+  </si>
+  <si>
+    <t>Arthur Avelar</t>
+  </si>
+  <si>
+    <t>Buscar Usuario</t>
+  </si>
+  <si>
+    <t>Remover Usuario</t>
+  </si>
+  <si>
+    <t>Editar Usuario</t>
+  </si>
+  <si>
+    <t>implementar no banco as modificaçoes</t>
+  </si>
+  <si>
+    <t>implementar cadastro de exercicios no backend (pesquisa, ediçao, cadastro, exclusão)</t>
+  </si>
+  <si>
+    <t>fazer a pagina do front do cadastro de exercicio(pesquisa, ediçao, cadastro, exclusão)</t>
+  </si>
+  <si>
+    <t>documentação</t>
+  </si>
+  <si>
+    <t>Ygor / Arthur Alexi</t>
+  </si>
+  <si>
+    <t>Marcos / Arthur Alexi
+(front e back)</t>
+  </si>
+  <si>
+    <t>Marcos / Arthur Alexi 
+(front e back)</t>
+  </si>
+  <si>
+    <t>implementar ficha de exercicio no backend (pesquisa, ediçao, cadastro, exclusão)</t>
+  </si>
+  <si>
+    <t>fazer a pagina do front da ficha de exercicio(pesquisa, ediçao, cadastro, exclusão, exibiçao para aluno e para admin)</t>
+  </si>
+  <si>
+    <t>7 e 8</t>
+  </si>
 </sst>
 </file>
 
@@ -725,7 +784,7 @@
     <numFmt numFmtId="164" formatCode="dd&quot;/&quot;mmm"/>
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mmm&quot;/&quot;yyyy&quot; &quot;"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -873,6 +932,10 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -6773,8 +6836,8 @@
   </sheetPr>
   <dimension ref="A1:R1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:G22"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10660,9 +10723,9 @@
   </sheetPr>
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12:F18"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10790,7 +10853,7 @@
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
       <c r="B7" s="71" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="72"/>
       <c r="D7" s="72"/>
@@ -10890,19 +10953,19 @@
         <v>2</v>
       </c>
       <c r="F11" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="G11" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="15" t="s">
+      <c r="I11" s="15">
+        <v>0</v>
+      </c>
+      <c r="J11" s="13" t="s">
         <v>86</v>
-      </c>
-      <c r="I11" s="15">
-        <v>0</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>87</v>
       </c>
       <c r="K11" s="3">
         <f t="shared" si="0"/>
@@ -10926,17 +10989,19 @@
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E12" s="14">
         <v>2</v>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="13" t="s">
+        <v>98</v>
+      </c>
       <c r="G12" s="54" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I12" s="15">
         <v>0</v>
@@ -10954,17 +11019,19 @@
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E13" s="14">
         <v>2</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>97</v>
+      </c>
       <c r="G13" s="54" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I13" s="15">
         <v>0</v>
@@ -10982,17 +11049,19 @@
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" s="14">
         <v>2</v>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="G14" s="54" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I14" s="15">
         <v>0</v>
@@ -11010,17 +11079,19 @@
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" s="14">
         <v>2</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>97</v>
+      </c>
       <c r="G15" s="54" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I15" s="15">
         <v>0</v>
@@ -11034,17 +11105,19 @@
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E16" s="14">
         <v>2</v>
       </c>
-      <c r="F16" s="14"/>
+      <c r="F16" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="G16" s="54" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I16" s="15">
         <v>0</v>
@@ -11058,17 +11131,19 @@
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E17" s="14">
         <v>2</v>
       </c>
-      <c r="F17" s="14"/>
+      <c r="F17" s="14" t="s">
+        <v>97</v>
+      </c>
       <c r="G17" s="54" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I17" s="15">
         <v>0</v>
@@ -11082,17 +11157,19 @@
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E18" s="14">
         <v>2</v>
       </c>
-      <c r="F18" s="14"/>
+      <c r="F18" s="14" t="s">
+        <v>97</v>
+      </c>
       <c r="G18" s="54" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I18" s="15">
         <v>0</v>
@@ -11105,10 +11182,18 @@
         <v>9</v>
       </c>
       <c r="C19" s="12"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="54"/>
+      <c r="D19" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="14">
+        <v>2</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="54" t="s">
+        <v>48</v>
+      </c>
       <c r="H19" s="15">
         <v>0</v>
       </c>
@@ -11879,13 +11964,13 @@
       <c r="C62" s="37"/>
       <c r="D62" s="37">
         <f>COUNTIFS(D11:D60, "&lt;&gt;"&amp;"")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E62" s="37"/>
       <c r="F62" s="37"/>
       <c r="G62" s="56">
         <f>COUNTIFS(G11:G60, "Concluído",D11:D60, "&lt;&gt;"&amp;"")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -13445,8 +13530,8 @@
   </sheetPr>
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -13664,10 +13749,18 @@
         <v>1</v>
       </c>
       <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="54"/>
+      <c r="D11" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="13">
+        <v>2</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>45</v>
+      </c>
       <c r="H11" s="15">
         <v>0</v>
       </c>
@@ -13696,10 +13789,18 @@
         <v>2</v>
       </c>
       <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="54"/>
+      <c r="D12" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="13">
+        <v>2</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G12" s="54" t="s">
+        <v>45</v>
+      </c>
       <c r="H12" s="15">
         <v>0</v>
       </c>
@@ -13718,10 +13819,18 @@
         <v>3</v>
       </c>
       <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="54"/>
+      <c r="D13" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G13" s="54" t="s">
+        <v>45</v>
+      </c>
       <c r="H13" s="15">
         <v>0</v>
       </c>
@@ -13740,10 +13849,18 @@
         <v>4</v>
       </c>
       <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="54"/>
+      <c r="D14" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="13">
+        <v>15</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="54" t="s">
+        <v>41</v>
+      </c>
       <c r="H14" s="15">
         <v>0</v>
       </c>
@@ -13756,16 +13873,24 @@
         <v>44829</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="11">
         <v>5</v>
       </c>
       <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="54"/>
+      <c r="D15" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="13">
+        <v>15</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="54" t="s">
+        <v>41</v>
+      </c>
       <c r="H15" s="15">
         <v>0</v>
       </c>
@@ -13781,10 +13906,18 @@
         <v>6</v>
       </c>
       <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="54"/>
+      <c r="D16" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="13">
+        <v>15</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="54" t="s">
+        <v>41</v>
+      </c>
       <c r="H16" s="15">
         <v>0</v>
       </c>
@@ -13800,10 +13933,18 @@
         <v>7</v>
       </c>
       <c r="C17" s="12"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="54"/>
+      <c r="D17" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="13">
+        <v>15</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" s="54" t="s">
+        <v>41</v>
+      </c>
       <c r="H17" s="15">
         <v>0</v>
       </c>
@@ -13819,10 +13960,18 @@
         <v>8</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="54"/>
+      <c r="D18" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="54" t="s">
+        <v>41</v>
+      </c>
       <c r="H18" s="15">
         <v>0</v>
       </c>
@@ -13832,16 +13981,24 @@
       <c r="J18" s="13"/>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="11">
         <v>9</v>
       </c>
       <c r="C19" s="12"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="54"/>
+      <c r="D19" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" s="54" t="s">
+        <v>41</v>
+      </c>
       <c r="H19" s="15">
         <v>0</v>
       </c>
@@ -13857,10 +14014,18 @@
         <v>10</v>
       </c>
       <c r="C20" s="12"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="54"/>
+      <c r="D20" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="54" t="s">
+        <v>41</v>
+      </c>
       <c r="H20" s="15">
         <v>0</v>
       </c>
@@ -13876,10 +14041,18 @@
         <v>11</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="54"/>
+      <c r="D21" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" s="54" t="s">
+        <v>41</v>
+      </c>
       <c r="H21" s="15">
         <v>0</v>
       </c>
@@ -14785,7 +14958,7 @@
       <c r="C71" s="37"/>
       <c r="D71" s="37">
         <f>COUNTIFS(D11:D60, "&lt;&gt;"&amp;"")</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E71" s="37"/>
       <c r="F71" s="37"/>
@@ -16238,6 +16411,7 @@
     <mergeCell ref="B75:G75"/>
     <mergeCell ref="B76:G76"/>
   </mergeCells>
+  <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="F20:F25">
     <cfRule type="expression" dxfId="205" priority="1">
       <formula>NOT(ISERROR(SEARCH(($B$74),(F20))))</formula>

</xml_diff>